<commit_message>
'Report' returned to its glory
Table printing is broken!!
</commit_message>
<xml_diff>
--- a/inst/extdata/description.xlsx
+++ b/inst/extdata/description.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_stuff\Martys_cookbook\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mrkmartongmailcom.sharepoint.com/sites/-/Shared Documents/General/Stats_R/R/MartysProjectTemplate/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="8_{003D5CBA-6A3A-438C-90F0-680B5A026A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DF53F7C-CBA3-4C77-B423-B440F55901C8}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DF53F7C-CBA3-4C77-B423-B440F55901C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -224,9 +224,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -264,7 +264,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -370,7 +370,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -512,7 +512,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -523,7 +523,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -675,8 +675,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd1a842694638f83c0368e938b836db">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94cc445afcc642aee4df2ae1f5e01e9e" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c475670649ec5cd3368ad2cdfcd3a78f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d0bd468940090131f35faadce84a875" ns2:_="" ns3:_="">
     <xsd:import namespace="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
     <xsd:import namespace="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
     <xsd:element name="properties">
@@ -699,6 +708,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -778,6 +788,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -895,19 +910,29 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a95d4ba5-ac50-4ccb-8f38-68d250b34105" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="3073c576-dbcc-4dca-a8e5-ccf7a0688d93">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF06E878-B30F-43EB-A425-6F4475635266}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FA154B-F08A-45A5-8BDA-4DFA67221AC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FA154B-F08A-45A5-8BDA-4DFA67221AC6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{20DE76E8-22AE-424A-890D-FDD19E3D2CDA}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B33E1018-8E59-443E-AAD7-4745B2F55AD6}"/>
 </file>
</xml_diff>

<commit_message>
Added enchanced way of setting gtsummary theme (doesnt crash idf lib. not loaded)
</commit_message>
<xml_diff>
--- a/inst/extdata/description.xlsx
+++ b/inst/extdata/description.xlsx
@@ -675,8 +675,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="5fd1a842694638f83c0368e938b836db">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="94cc445afcc642aee4df2ae1f5e01e9e" ns2:_="" ns3:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F0ADBC3A86B10A4085B52F181C274AA0" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="c475670649ec5cd3368ad2cdfcd3a78f">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="3073c576-dbcc-4dca-a8e5-ccf7a0688d93" xmlns:ns3="a95d4ba5-ac50-4ccb-8f38-68d250b34105" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4d0bd468940090131f35faadce84a875" ns2:_="" ns3:_="">
     <xsd:import namespace="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
     <xsd:import namespace="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
     <xsd:element name="properties">
@@ -699,6 +699,7 @@
                 <xsd:element ref="ns3:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -778,6 +779,11 @@
     <xsd:element name="MediaServiceSearchProperties" ma:index="22" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="23" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -905,7 +911,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EF06E878-B30F-43EB-A425-6F4475635266}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783B5A75-FC2C-4383-A1C4-78233379F2FC}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
Wrangling better handling mpl sheets
</commit_message>
<xml_diff>
--- a/inst/extdata/description.xlsx
+++ b/inst/extdata/description.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\R_stuff\Martys_cookbook\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c770e11f011a8c48/DKM/Válallkozás/TMC/TMC.KolumbanErika.RCT/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{003D5CBA-6A3A-438C-90F0-680B5A026A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="8_{003D5CBA-6A3A-438C-90F0-680B5A026A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0773E0-552A-4EEA-AA20-C5F4C7CCE4E1}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5DF53F7C-CBA3-4C77-B423-B440F55901C8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5DF53F7C-CBA3-4C77-B423-B440F55901C8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -23,9 +23,12 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="32">
   <si>
     <t>col.ID</t>
   </si>
@@ -117,6 +120,18 @@
   </si>
   <si>
     <t>This is a date column to illustrate transformations</t>
+  </si>
+  <si>
+    <t>Sheet</t>
+  </si>
+  <si>
+    <t>Data</t>
+  </si>
+  <si>
+    <t>Data (2)</t>
+  </si>
+  <si>
+    <t>Data (3)</t>
   </si>
 </sst>
 </file>
@@ -223,10 +238,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -264,7 +283,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -370,7 +389,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -512,165 +531,464 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D1AB551-227B-45B9-A532-95770313E0F2}">
-  <dimension ref="A1:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8ABE5619-AA6D-467A-9003-D71F5C0412FF}">
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.5703125" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>10</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>16</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>12</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>14</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="C7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>16</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>19</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>17</v>
+      </c>
+      <c r="F11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>17</v>
+      </c>
+      <c r="F12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>5</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" t="s">
+        <v>17</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
+        <v>15</v>
+      </c>
+      <c r="E14" t="s">
+        <v>16</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>31</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>17</v>
+      </c>
+      <c r="F17" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>12</v>
+      </c>
+      <c r="E18" t="s">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
+        <v>15</v>
+      </c>
+      <c r="E21" t="s">
+        <v>16</v>
+      </c>
+      <c r="F21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>31</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" t="s">
         <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -911,9 +1229,28 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783B5A75-FC2C-4383-A1C4-78233379F2FC}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{783B5A75-FC2C-4383-A1C4-78233379F2FC}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="3073c576-dbcc-4dca-a8e5-ccf7a0688d93"/>
+    <ds:schemaRef ds:uri="a95d4ba5-ac50-4ccb-8f38-68d250b34105"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FA154B-F08A-45A5-8BDA-4DFA67221AC6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{92FA154B-F08A-45A5-8BDA-4DFA67221AC6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>